<commit_message>
added contingency awareness test
</commit_message>
<xml_diff>
--- a/conditions3.xlsx
+++ b/conditions3.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="55">
   <si>
     <t>position</t>
   </si>
@@ -154,6 +154,42 @@
   </si>
   <si>
     <t xml:space="preserve">To use this conditions file, change the aux1 values by randomising the rand_num column. Then select aux1 and rand_num from the first to the 5th row and sort. All the other values should update according to this new randomisation. </t>
+  </si>
+  <si>
+    <t>min</t>
+  </si>
+  <si>
+    <t>trial</t>
+  </si>
+  <si>
+    <t>rep</t>
+  </si>
+  <si>
+    <t>u1</t>
+  </si>
+  <si>
+    <t>u2</t>
+  </si>
+  <si>
+    <t>o1</t>
+  </si>
+  <si>
+    <t>o2</t>
+  </si>
+  <si>
+    <t>days</t>
+  </si>
+  <si>
+    <t>TOTAL</t>
+  </si>
+  <si>
+    <t>total/day</t>
+  </si>
+  <si>
+    <t>total 2 days</t>
+  </si>
+  <si>
+    <t>total/resp/day</t>
   </si>
 </sst>
 </file>
@@ -587,14 +623,14 @@
         <v>30</v>
       </c>
       <c r="F2">
-        <v>120</v>
+        <v>180</v>
       </c>
       <c r="G2" t="s">
         <v>26</v>
       </c>
       <c r="H2">
         <f ca="1">RAND()</f>
-        <v>0.7682293682561121</v>
+        <v>9.3830183549828527E-2</v>
       </c>
       <c r="I2" t="s">
         <v>41</v>
@@ -635,14 +671,14 @@
         <v>31</v>
       </c>
       <c r="F3">
-        <v>120</v>
+        <v>180</v>
       </c>
       <c r="G3" t="s">
         <v>29</v>
       </c>
       <c r="H3">
         <f ca="1">RAND()</f>
-        <v>0.861962516188578</v>
+        <v>0.86563474722878764</v>
       </c>
       <c r="I3" t="s">
         <v>41</v>
@@ -683,14 +719,14 @@
         <v>31</v>
       </c>
       <c r="F4">
-        <v>300</v>
+        <v>330</v>
       </c>
       <c r="G4" t="s">
         <v>28</v>
       </c>
       <c r="H4">
         <f ca="1">RAND()</f>
-        <v>0.75297493060356346</v>
+        <v>6.2712304150263076E-2</v>
       </c>
       <c r="I4" t="s">
         <v>41</v>
@@ -731,14 +767,14 @@
         <v>30</v>
       </c>
       <c r="F5">
-        <v>300</v>
+        <v>330</v>
       </c>
       <c r="G5" t="s">
         <v>27</v>
       </c>
       <c r="H5">
         <f ca="1">RAND()</f>
-        <v>0.83027784074498234</v>
+        <v>0.20658979285619083</v>
       </c>
       <c r="I5" t="s">
         <v>41</v>
@@ -781,7 +817,7 @@
         <v>stim/gold_coin.png</v>
       </c>
       <c r="F6">
-        <v>300</v>
+        <v>330</v>
       </c>
       <c r="G6" t="str">
         <f>VLOOKUP(A6,$A$2:$G$5,7,0)</f>
@@ -828,7 +864,7 @@
         <v>stim/silver_coin.png</v>
       </c>
       <c r="F7">
-        <v>300</v>
+        <v>330</v>
       </c>
       <c r="G7" t="str">
         <f t="shared" ref="G7" si="8">VLOOKUP(A7,$A$2:$G$5,7,0)</f>
@@ -1016,17 +1052,220 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:L14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="8" max="8" width="11" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>42</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>44</v>
+      </c>
+      <c r="B6" t="s">
+        <v>43</v>
+      </c>
+      <c r="C6" t="s">
+        <v>45</v>
+      </c>
+      <c r="D6" t="s">
+        <v>54</v>
+      </c>
+      <c r="E6" t="s">
+        <v>50</v>
+      </c>
+      <c r="F6" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>46</v>
+      </c>
+      <c r="B7">
+        <f>conditions!F2/60</f>
+        <v>3</v>
+      </c>
+      <c r="C7">
+        <v>2</v>
+      </c>
+      <c r="D7">
+        <f>B7*C7</f>
+        <v>6</v>
+      </c>
+      <c r="E7">
+        <v>2</v>
+      </c>
+      <c r="F7">
+        <f>E7*D7</f>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>47</v>
+      </c>
+      <c r="B8">
+        <f>conditions!F3/60</f>
+        <v>3</v>
+      </c>
+      <c r="C8">
+        <v>2</v>
+      </c>
+      <c r="D8">
+        <f>B8*C8</f>
+        <v>6</v>
+      </c>
+      <c r="E8">
+        <v>2</v>
+      </c>
+      <c r="F8">
+        <f t="shared" ref="F8:F12" si="0">E8*D8</f>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>48</v>
+      </c>
+      <c r="B9">
+        <f>conditions!F4/60</f>
+        <v>5.5</v>
+      </c>
+      <c r="C9">
+        <v>2</v>
+      </c>
+      <c r="D9">
+        <f>B9*C9</f>
+        <v>11</v>
+      </c>
+      <c r="E9">
+        <v>2</v>
+      </c>
+      <c r="F9">
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>49</v>
+      </c>
+      <c r="B10">
+        <f>conditions!F5/60</f>
+        <v>5.5</v>
+      </c>
+      <c r="C10">
+        <v>2</v>
+      </c>
+      <c r="D10">
+        <f>B10*C10</f>
+        <v>11</v>
+      </c>
+      <c r="E10">
+        <v>2</v>
+      </c>
+      <c r="F10">
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>48</v>
+      </c>
+      <c r="B11">
+        <f>conditions!F6/60</f>
+        <v>5.5</v>
+      </c>
+      <c r="C11">
+        <v>2</v>
+      </c>
+      <c r="D11">
+        <f>B11*C11</f>
+        <v>11</v>
+      </c>
+      <c r="E11">
+        <v>2</v>
+      </c>
+      <c r="F11">
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>49</v>
+      </c>
+      <c r="B12">
+        <f>conditions!F7/60</f>
+        <v>5.5</v>
+      </c>
+      <c r="C12">
+        <v>2</v>
+      </c>
+      <c r="D12">
+        <f>B12*C12</f>
+        <v>11</v>
+      </c>
+      <c r="E12">
+        <v>2</v>
+      </c>
+      <c r="F12">
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
+      <c r="I12" t="s">
+        <v>46</v>
+      </c>
+      <c r="J12" t="s">
+        <v>47</v>
+      </c>
+      <c r="K12" t="s">
+        <v>48</v>
+      </c>
+      <c r="L12" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="H13" t="s">
+        <v>53</v>
+      </c>
+      <c r="I13">
+        <f>+F7</f>
+        <v>12</v>
+      </c>
+      <c r="J13">
+        <f>F8</f>
+        <v>12</v>
+      </c>
+      <c r="K13">
+        <f>SUM(F9:F10)</f>
+        <v>44</v>
+      </c>
+      <c r="L13">
+        <f>SUM(F11:F12)</f>
+        <v>44</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C14" t="s">
+        <v>52</v>
+      </c>
+      <c r="D14">
+        <f>SUM(D7:D12)</f>
+        <v>56</v>
       </c>
     </row>
   </sheetData>

</xml_diff>